<commit_message>
Fix : EnemyDB 내용 수정
EnemyDB : DropItemID 삭제 , DropDia , AttackDistance 카테고리 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/Utill/ExcelToJsonWizard.v1.0.6/excel_files/EnemyDB.xlsx
+++ b/Assets/Resources/Utill/ExcelToJsonWizard.v1.0.6/excel_files/EnemyDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONG\Desktop\개발\TIL\20241126\외부데이터로드\ExcelToJsonWizard.v1.0.6\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\Utill\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820EA6C9-AFCC-49DB-A26D-B3D28274F406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DBC3CD-B52B-4A34-93CC-5B8687010E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD5DF776-12D7-4429-A84B-E30D2AE72BA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD5DF776-12D7-4429-A84B-E30D2AE72BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="EnemyDB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Descripton</t>
   </si>
   <si>
-    <t>DropItemID</t>
-  </si>
-  <si>
     <t>DropGold</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>List&lt;int&gt;</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -119,10 +113,6 @@
   </si>
   <si>
     <t>독사 설명</t>
-  </si>
-  <si>
-    <t>2000,2001,1000,1000</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
@@ -130,6 +120,22 @@
   </si>
   <si>
     <t>key</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DropDia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackDistance</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -732,11 +738,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1117,104 +1120,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A27B477-FBF8-4BE6-960A-9658697B848B}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1228,45 +1238,48 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
       <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5000</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1275,36 +1288,39 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5001</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>150</v>
       </c>
       <c r="E5">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -1313,36 +1329,39 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5002</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
       </c>
       <c r="E6">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1354,33 +1373,36 @@
         <v>5</v>
       </c>
       <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5003</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>250</v>
       </c>
       <c r="E7">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -1392,33 +1414,36 @@
         <v>5</v>
       </c>
       <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
         <v>0.8</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5004</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
       </c>
       <c r="E8">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -1427,36 +1452,39 @@
         <v>1</v>
       </c>
       <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
         <v>10</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.8</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5005</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>350</v>
       </c>
       <c r="E9">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1465,36 +1493,39 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>0.8</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>30</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
       <c r="L9">
         <v>0</v>
       </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5006</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1503,36 +1534,39 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>1.2</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>50</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
       <c r="L10">
         <v>0</v>
       </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5007</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1541,36 +1575,39 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>1.2</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>100</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
       <c r="L11">
         <v>0</v>
       </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5008</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1579,18 +1616,21 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>1.2</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>30</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
       <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>0</v>
       </c>
     </row>

</xml_diff>